<commit_message>
work on writer beg
</commit_message>
<xml_diff>
--- a/src/FileContainer/TpriceList.xlsx
+++ b/src/FileContainer/TpriceList.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="134">
   <si>
     <t>Keys</t>
   </si>
@@ -79,18 +79,12 @@
     <t>PRACTICE BALLS (V1 &amp; V1X) Loose</t>
   </si>
   <si>
-    <t>PRACTICE BALLS Pro V1 Practice Custom Dz 100PK</t>
-  </si>
-  <si>
     <t>PRACTICE BALLS NXT</t>
   </si>
   <si>
     <t>PRACTICE BALLS NXT - LOGO</t>
   </si>
   <si>
-    <t>NXT Practice Yellow</t>
-  </si>
-  <si>
     <t>716 AP1</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>2017 T-MB Steel</t>
   </si>
   <si>
-    <t>2017 T-MB Graphite</t>
-  </si>
-  <si>
     <t>Vokey SM6 - Tour Chrome</t>
   </si>
   <si>
@@ -148,15 +139,6 @@
     <t xml:space="preserve">Drivers  917 D2  </t>
   </si>
   <si>
-    <t xml:space="preserve">Drivers  917 D3  </t>
-  </si>
-  <si>
-    <t>Fairways  917 F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairways  917 F3  </t>
-  </si>
-  <si>
     <t>Cameron Crown 33"</t>
   </si>
   <si>
@@ -241,9 +223,6 @@
     <t>Flag Q Max (Dozen) (FRA/BEL/SPA/POR/SWE)</t>
   </si>
   <si>
-    <t>Flag Q Max (1/2 dz) (ENG/SCO/EIR/NIR/WAL/SA/GER/NL/CH)</t>
-  </si>
-  <si>
     <t>NEW! Tour Performance (Dozen)</t>
   </si>
   <si>
@@ -256,9 +235,6 @@
     <t>NEW! Two Tone Mesh (Dozen)</t>
   </si>
   <si>
-    <t xml:space="preserve">Flat Bill - Black/White (1/2 dz) </t>
-  </si>
-  <si>
     <t>NEW! Ladies Pink Ribbon Visor (1/2 dz)</t>
   </si>
   <si>
@@ -271,24 +247,9 @@
     <t>NEW! Junior Performance Cap (1/2 dz)</t>
   </si>
   <si>
-    <t>Sta Dry Bucket (1/2 dz)</t>
-  </si>
-  <si>
-    <t>Sta Dry Cap (1/2 dz)</t>
-  </si>
-  <si>
-    <t>NEW! Winter POM POM (1/2 dz)</t>
-  </si>
-  <si>
     <t>NEW! Winter Fitted Beanie (Striped) Ladies and Mens (1/2 dz)</t>
   </si>
   <si>
-    <t>NEW! Winter Jacquard Beanie (1/2 dz)</t>
-  </si>
-  <si>
-    <t>NEW! Performance Snood (1/2 dz)</t>
-  </si>
-  <si>
     <t>Performance Beanie (1/2 dz)</t>
   </si>
   <si>
@@ -328,12 +289,6 @@
     <t>PROFESSIONAL Briefcase</t>
   </si>
   <si>
-    <t>PROFESSIONAL Zippered Dopp Kit</t>
-  </si>
-  <si>
-    <t>PROFESSIONAL Tote Bag</t>
-  </si>
-  <si>
     <t>ESSENTIAL Travel Cover</t>
   </si>
   <si>
@@ -373,9 +328,6 @@
     <t>Microfibre Towel</t>
   </si>
   <si>
-    <t>Dri-Hood Towel</t>
-  </si>
-  <si>
     <t>NEW! Microfibre Tri-Fold Cart Towel</t>
   </si>
   <si>
@@ -385,24 +337,6 @@
     <t>Black Leather Headcover - Fairway</t>
   </si>
   <si>
-    <t>Black Leather Headcover - Hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW! Leather White Headcover - Driver </t>
-  </si>
-  <si>
-    <t>NEW! Leather White Headcover - Fairway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW! Leather White Headcover - Hybrid </t>
-  </si>
-  <si>
-    <t>Scotty Cameron Headcover</t>
-  </si>
-  <si>
-    <t>Hand Warmer</t>
-  </si>
-  <si>
     <t>Ear Band</t>
   </si>
   <si>
@@ -430,12 +364,6 @@
     <t>acc</t>
   </si>
   <si>
-    <t>716 AP1 Forged</t>
-  </si>
-  <si>
-    <t>716 AP1 Forged Graphite</t>
-  </si>
-  <si>
     <t>2017 AP1 Steel</t>
   </si>
   <si>
@@ -448,33 +376,18 @@
     <t>2017 AP2 Graphite</t>
   </si>
   <si>
-    <t>2017 AP3 Steel</t>
-  </si>
-  <si>
-    <t>2017 AP3 Graphite</t>
-  </si>
-  <si>
     <t>2017 CB Steel</t>
   </si>
   <si>
-    <t>2017 CB Graphite</t>
-  </si>
-  <si>
     <t>2017 MB Steel</t>
   </si>
   <si>
-    <t>2017 MB Graphite</t>
-  </si>
-  <si>
     <t>Hybrids - 818H1</t>
   </si>
   <si>
     <t>Hybrids - 818H2</t>
   </si>
   <si>
-    <t>Drivers  917 D4</t>
-  </si>
-  <si>
     <t xml:space="preserve">bags </t>
   </si>
   <si>
@@ -493,16 +406,25 @@
     <t>hdv</t>
   </si>
   <si>
-    <t>AGDISC1</t>
+    <t xml:space="preserve">Drivers  917 D7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairways  917 F  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairways  917 FD   </t>
+  </si>
+  <si>
+    <t>NEW! Winter POM POM Beanie (1/2 dz)</t>
+  </si>
+  <si>
+    <t>TRADEZR1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -532,9 +454,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,11 +757,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -849,1641 +768,1366 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>25.7</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>25.7</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>17.04</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>12.85</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>10.37</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>7.28</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>7.28</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>5.95</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>6.25</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>6.25</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>7.3</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>7.3</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>14.5</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>3.5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>15</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>6.4</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>18.3</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21">
-        <v>18.3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22">
-        <v>8.6</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24">
-        <v>8.6</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25">
-        <v>52.92</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26">
-        <v>62.72</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>66.64</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30">
-        <v>76.44</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>66.64</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>66.64</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="C33">
-        <v>98</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="C34">
-        <v>107.8</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="C35">
-        <v>76.44</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="C36">
-        <v>76.44</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="C37">
-        <v>60.76</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C38">
-        <v>70.56</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="C39">
-        <v>76.44</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="C40">
-        <v>86.24</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="C41">
-        <v>70.56</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>76.44</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>70.56</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="C44">
-        <v>76.44</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C45">
-        <v>70.56</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="C46">
-        <v>76.44</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C47">
-        <v>122.5</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C48">
-        <v>132.30000000000001</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C49">
-        <v>68.599999999999994</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="C50">
-        <v>68.599999999999994</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C51">
-        <v>68.599999999999994</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C52">
-        <v>79.38</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53">
-        <v>114.66</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C54">
-        <v>114.66</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="C55">
-        <v>132.30000000000001</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
       <c r="C56">
-        <v>132.30000000000001</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C57">
-        <v>245</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C58">
-        <v>245</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C60">
-        <v>151.9</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C61">
-        <v>151.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C62">
-        <v>181.3</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C63">
-        <v>191.1</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C64">
-        <v>181.3</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C65">
-        <v>181.3</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C69">
-        <v>343</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C70">
-        <v>308.7</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C71">
-        <v>5.88</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C72">
-        <v>9.25</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C73">
-        <v>7.94</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C74">
-        <v>7.1</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="C75">
-        <v>183.26</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C76">
-        <v>99.96</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="C77">
-        <v>108.29</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C78">
-        <v>79.14</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
         <v>63</v>
       </c>
       <c r="C79">
-        <v>62.48</v>
+        <v>900</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
         <v>64</v>
       </c>
       <c r="C80">
-        <v>95.8</v>
+        <v>600</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
       </c>
       <c r="C81">
-        <v>95.8</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B82" t="s">
         <v>66</v>
       </c>
       <c r="C82">
-        <v>83.3</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>67</v>
       </c>
       <c r="C83">
-        <v>83.3</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B84" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C84">
-        <v>69.14</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="C85">
-        <v>69.14</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B86" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C86">
-        <v>83.3</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="C87">
-        <v>58.31</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="C88">
-        <v>58.31</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C89">
-        <v>33.32</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C90">
-        <v>24.99</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C91">
-        <v>105.84</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C92">
-        <v>102</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B94" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C94">
-        <v>51.82</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C95">
-        <v>103.64</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B96" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C96">
-        <v>83.79</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C98">
-        <v>103.64</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C99">
-        <v>51.82</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B100" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C100">
-        <v>51.82</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C101">
-        <v>57.33</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C102">
-        <v>51.82</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C103">
-        <v>51.82</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C104">
-        <v>74.97</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B105" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C105">
-        <v>66.64</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B106" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C106">
-        <v>43.73</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C107">
-        <v>43.73</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C108">
-        <v>49.98</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B109" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C109">
-        <v>43.73</v>
+        <v>800</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B110" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C110">
-        <v>43.73</v>
+        <v>800</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C113">
-        <v>103.64</v>
+        <v>700</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C114">
-        <v>103.64</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C115">
-        <v>114.66</v>
+        <v>600</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C116">
-        <v>99.23</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C117">
-        <v>99.23</v>
+        <v>300</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C118">
-        <v>74.97</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C119">
-        <v>70.56</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B120" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C120">
-        <v>74.97</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B121" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C121">
-        <v>70.56</v>
+        <v>550</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B122" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C122">
-        <v>74.97</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B123" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C123">
-        <v>26.46</v>
+        <v>90</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B124" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>136</v>
-      </c>
-      <c r="B125" t="s">
-        <v>105</v>
-      </c>
-      <c r="C125">
-        <v>64.39</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>136</v>
-      </c>
-      <c r="B126" t="s">
-        <v>106</v>
-      </c>
-      <c r="C126">
-        <v>52.92</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>136</v>
-      </c>
-      <c r="B127" t="s">
-        <v>107</v>
-      </c>
-      <c r="C127">
-        <v>32.630000000000003</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>136</v>
-      </c>
-      <c r="B128" t="s">
-        <v>108</v>
-      </c>
-      <c r="C128">
-        <v>32.630000000000003</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>136</v>
-      </c>
-      <c r="B129" t="s">
-        <v>109</v>
-      </c>
-      <c r="C129">
-        <v>9.26</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>136</v>
-      </c>
-      <c r="B130" t="s">
-        <v>110</v>
-      </c>
-      <c r="C130">
-        <v>4.63</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>136</v>
-      </c>
-      <c r="B131" t="s">
-        <v>111</v>
-      </c>
-      <c r="C131">
-        <v>35.28</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>136</v>
-      </c>
-      <c r="B132" t="s">
-        <v>112</v>
-      </c>
-      <c r="C132">
-        <v>44.1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>136</v>
-      </c>
-      <c r="B133" t="s">
-        <v>113</v>
-      </c>
-      <c r="C133">
-        <v>22.05</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>136</v>
-      </c>
-      <c r="B134" t="s">
-        <v>114</v>
-      </c>
-      <c r="C134">
-        <v>48.51</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>136</v>
-      </c>
-      <c r="B135" t="s">
-        <v>115</v>
-      </c>
-      <c r="C135">
-        <v>11.47</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>136</v>
-      </c>
-      <c r="B136" t="s">
-        <v>116</v>
-      </c>
-      <c r="C136">
-        <v>9.26</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>136</v>
-      </c>
-      <c r="B137" t="s">
-        <v>117</v>
-      </c>
-      <c r="C137">
-        <v>9.26</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>136</v>
-      </c>
-      <c r="B138" t="s">
-        <v>118</v>
-      </c>
-      <c r="C138">
-        <v>15.44</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>136</v>
-      </c>
-      <c r="B139" t="s">
-        <v>119</v>
-      </c>
-      <c r="C139">
-        <v>6.62</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>136</v>
-      </c>
-      <c r="B140" t="s">
-        <v>120</v>
-      </c>
-      <c r="C140">
-        <v>28.22</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>136</v>
-      </c>
-      <c r="B141" t="s">
-        <v>121</v>
-      </c>
-      <c r="C141">
-        <v>26.46</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>136</v>
-      </c>
-      <c r="B142" t="s">
-        <v>122</v>
-      </c>
-      <c r="C142">
-        <v>23.81</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>136</v>
-      </c>
-      <c r="B143" t="s">
-        <v>123</v>
-      </c>
-      <c r="C143">
-        <v>28.22</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>136</v>
-      </c>
-      <c r="B144" t="s">
-        <v>124</v>
-      </c>
-      <c r="C144">
-        <v>26.46</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>136</v>
-      </c>
-      <c r="B145" t="s">
-        <v>125</v>
-      </c>
-      <c r="C145">
-        <v>23.81</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>136</v>
-      </c>
-      <c r="B146" t="s">
-        <v>126</v>
-      </c>
-      <c r="C146" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>136</v>
-      </c>
-      <c r="B147" t="s">
-        <v>127</v>
-      </c>
-      <c r="C147">
-        <v>15.83</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>136</v>
-      </c>
-      <c r="B148" t="s">
-        <v>128</v>
-      </c>
-      <c r="C148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>136</v>
-      </c>
-      <c r="B149" t="s">
-        <v>129</v>
-      </c>
-      <c r="C149">
-        <v>12.5</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>